<commit_message>
feat(Snakefile): new improvement for Strelka DNM calls
</commit_message>
<xml_diff>
--- a/cgr_summary.xlsx
+++ b/cgr_summary.xlsx
@@ -46,6 +46,309 @@
     <t>JIGV_Strelka</t>
   </si>
   <si>
+    <t>t0007</t>
+  </si>
+  <si>
+    <t>t0007c1</t>
+  </si>
+  <si>
+    <t>SC499427</t>
+  </si>
+  <si>
+    <t>SC499423</t>
+  </si>
+  <si>
+    <t>SC499428</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>JIGV HTML</t>
+  </si>
+  <si>
+    <t>t0617</t>
+  </si>
+  <si>
+    <t>t0617c1</t>
+  </si>
+  <si>
+    <t>SC260701</t>
+  </si>
+  <si>
+    <t>SC260705</t>
+  </si>
+  <si>
+    <t>SC260697</t>
+  </si>
+  <si>
+    <t>t0243</t>
+  </si>
+  <si>
+    <t>t0243c1</t>
+  </si>
+  <si>
+    <t>SC736787</t>
+  </si>
+  <si>
+    <t>SC736702</t>
+  </si>
+  <si>
+    <t>SC736772</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>t0058</t>
+  </si>
+  <si>
+    <t>t0058c1</t>
+  </si>
+  <si>
+    <t>SC109341</t>
+  </si>
+  <si>
+    <t>SC109353</t>
+  </si>
+  <si>
+    <t>SC109336</t>
+  </si>
+  <si>
+    <t>t0712</t>
+  </si>
+  <si>
+    <t>t0712c1</t>
+  </si>
+  <si>
+    <t>SC742313</t>
+  </si>
+  <si>
+    <t>SC742314</t>
+  </si>
+  <si>
+    <t>SC742315</t>
+  </si>
+  <si>
+    <t>t0565</t>
+  </si>
+  <si>
+    <t>t0565c2</t>
+  </si>
+  <si>
+    <t>SC109437</t>
+  </si>
+  <si>
+    <t>SC109373</t>
+  </si>
+  <si>
+    <t>SC109368</t>
+  </si>
+  <si>
+    <t>t0693</t>
+  </si>
+  <si>
+    <t>t0693c2</t>
+  </si>
+  <si>
+    <t>SC742220</t>
+  </si>
+  <si>
+    <t>SC742221</t>
+  </si>
+  <si>
+    <t>SC742222</t>
+  </si>
+  <si>
+    <t>t0058c2</t>
+  </si>
+  <si>
+    <t>SC108472</t>
+  </si>
+  <si>
+    <t>t0565c1</t>
+  </si>
+  <si>
+    <t>SC109438</t>
+  </si>
+  <si>
+    <t>t0760</t>
+  </si>
+  <si>
+    <t>t0760c1</t>
+  </si>
+  <si>
+    <t>SC736729</t>
+  </si>
+  <si>
+    <t>SC736824</t>
+  </si>
+  <si>
+    <t>SC736803</t>
+  </si>
+  <si>
+    <t>t0592</t>
+  </si>
+  <si>
+    <t>t0592c1</t>
+  </si>
+  <si>
+    <t>SC109501</t>
+  </si>
+  <si>
+    <t>SC109499</t>
+  </si>
+  <si>
+    <t>SC109498</t>
+  </si>
+  <si>
+    <t>t0750</t>
+  </si>
+  <si>
+    <t>t0750c1</t>
+  </si>
+  <si>
+    <t>SC736755</t>
+  </si>
+  <si>
+    <t>SC736760</t>
+  </si>
+  <si>
+    <t>SC736736</t>
+  </si>
+  <si>
+    <t>t0707</t>
+  </si>
+  <si>
+    <t>t0707c1</t>
+  </si>
+  <si>
+    <t>SC742305</t>
+  </si>
+  <si>
+    <t>SC742306</t>
+  </si>
+  <si>
+    <t>SC742307</t>
+  </si>
+  <si>
+    <t>t0600</t>
+  </si>
+  <si>
+    <t>t0600c1</t>
+  </si>
+  <si>
+    <t>SC109494</t>
+  </si>
+  <si>
+    <t>SC109514</t>
+  </si>
+  <si>
+    <t>SC109500</t>
+  </si>
+  <si>
+    <t>t0140</t>
+  </si>
+  <si>
+    <t>t0140c1</t>
+  </si>
+  <si>
+    <t>SC742196</t>
+  </si>
+  <si>
+    <t>SC742286</t>
+  </si>
+  <si>
+    <t>SC742197</t>
+  </si>
+  <si>
+    <t>t0315</t>
+  </si>
+  <si>
+    <t>t0315c2</t>
+  </si>
+  <si>
+    <t>SC260715</t>
+  </si>
+  <si>
+    <t>SC260727</t>
+  </si>
+  <si>
+    <t>SC260729</t>
+  </si>
+  <si>
+    <t>t0599</t>
+  </si>
+  <si>
+    <t>t0599c1</t>
+  </si>
+  <si>
+    <t>SC736788</t>
+  </si>
+  <si>
+    <t>SC736742</t>
+  </si>
+  <si>
+    <t>SC736743</t>
+  </si>
+  <si>
+    <t>t0623</t>
+  </si>
+  <si>
+    <t>t0623c1</t>
+  </si>
+  <si>
+    <t>SC253881</t>
+  </si>
+  <si>
+    <t>SC253893</t>
+  </si>
+  <si>
+    <t>SC253894</t>
+  </si>
+  <si>
+    <t>t0600c2</t>
+  </si>
+  <si>
+    <t>SC109495</t>
+  </si>
+  <si>
+    <t>t0315c1</t>
+  </si>
+  <si>
+    <t>SC260714</t>
+  </si>
+  <si>
+    <t>t0209</t>
+  </si>
+  <si>
+    <t>t0209c1</t>
+  </si>
+  <si>
+    <t>SC742216</t>
+  </si>
+  <si>
+    <t>SC742271</t>
+  </si>
+  <si>
+    <t>SC742272</t>
+  </si>
+  <si>
+    <t>t0703</t>
+  </si>
+  <si>
+    <t>t0703c1</t>
+  </si>
+  <si>
+    <t>SC742295</t>
+  </si>
+  <si>
+    <t>SC742296</t>
+  </si>
+  <si>
+    <t>SC742297</t>
+  </si>
+  <si>
     <t>t0666</t>
   </si>
   <si>
@@ -61,172 +364,190 @@
     <t>SC502234</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>JIGV HTML</t>
-  </si>
-  <si>
-    <t>t0315</t>
-  </si>
-  <si>
-    <t>t0315c1</t>
-  </si>
-  <si>
-    <t>SC260714</t>
-  </si>
-  <si>
-    <t>SC260727</t>
-  </si>
-  <si>
-    <t>SC260729</t>
-  </si>
-  <si>
-    <t>t0140</t>
-  </si>
-  <si>
-    <t>t0140c1</t>
-  </si>
-  <si>
-    <t>SC742196</t>
-  </si>
-  <si>
-    <t>SC742286</t>
-  </si>
-  <si>
-    <t>SC742197</t>
-  </si>
-  <si>
-    <t>t0565</t>
-  </si>
-  <si>
-    <t>t0565c2</t>
-  </si>
-  <si>
-    <t>SC109437</t>
-  </si>
-  <si>
-    <t>SC109373</t>
-  </si>
-  <si>
-    <t>SC109368</t>
+    <t>t0594</t>
+  </si>
+  <si>
+    <t>t0594c1</t>
+  </si>
+  <si>
+    <t>SC736817</t>
+  </si>
+  <si>
+    <t>SC736753</t>
+  </si>
+  <si>
+    <t>SC736754</t>
+  </si>
+  <si>
+    <t>t0271</t>
+  </si>
+  <si>
+    <t>t0271c1</t>
+  </si>
+  <si>
+    <t>SC109417</t>
+  </si>
+  <si>
+    <t>SC109426</t>
+  </si>
+  <si>
+    <t>SC109450</t>
+  </si>
+  <si>
+    <t>t0022</t>
+  </si>
+  <si>
+    <t>t0022c1</t>
+  </si>
+  <si>
+    <t>SC742290</t>
+  </si>
+  <si>
+    <t>SC742217</t>
+  </si>
+  <si>
+    <t>SC742218</t>
+  </si>
+  <si>
+    <t>t0280</t>
+  </si>
+  <si>
+    <t>t0280c1</t>
+  </si>
+  <si>
+    <t>SC109512</t>
+  </si>
+  <si>
+    <t>SC109516</t>
+  </si>
+  <si>
+    <t>SC109507</t>
   </si>
   <si>
     <t>t0575</t>
   </si>
   <si>
+    <t>t0575c2</t>
+  </si>
+  <si>
+    <t>SC109406</t>
+  </si>
+  <si>
+    <t>SC109395</t>
+  </si>
+  <si>
+    <t>SC109405</t>
+  </si>
+  <si>
+    <t>t0766</t>
+  </si>
+  <si>
+    <t>t0766c1</t>
+  </si>
+  <si>
+    <t>SC742179</t>
+  </si>
+  <si>
+    <t>SC736703</t>
+  </si>
+  <si>
+    <t>SC730933</t>
+  </si>
+  <si>
+    <t>t0042</t>
+  </si>
+  <si>
+    <t>t0042c1</t>
+  </si>
+  <si>
+    <t>SC253873</t>
+  </si>
+  <si>
+    <t>SC253877</t>
+  </si>
+  <si>
+    <t>SC253872</t>
+  </si>
+  <si>
+    <t>t0739</t>
+  </si>
+  <si>
+    <t>t0739c1</t>
+  </si>
+  <si>
+    <t>SC736720</t>
+  </si>
+  <si>
+    <t>SC736795</t>
+  </si>
+  <si>
+    <t>SC736726</t>
+  </si>
+  <si>
+    <t>t0679</t>
+  </si>
+  <si>
+    <t>t0679c2</t>
+  </si>
+  <si>
+    <t>SC742276</t>
+  </si>
+  <si>
+    <t>SC742188</t>
+  </si>
+  <si>
+    <t>SC742277</t>
+  </si>
+  <si>
+    <t>t0705</t>
+  </si>
+  <si>
+    <t>t0705c1</t>
+  </si>
+  <si>
+    <t>SC742298</t>
+  </si>
+  <si>
+    <t>SC742301</t>
+  </si>
+  <si>
+    <t>SC742299</t>
+  </si>
+  <si>
+    <t>t0765</t>
+  </si>
+  <si>
+    <t>t0765c1</t>
+  </si>
+  <si>
+    <t>SC736700</t>
+  </si>
+  <si>
+    <t>SC736738</t>
+  </si>
+  <si>
+    <t>SC736739</t>
+  </si>
+  <si>
     <t>t0575c1</t>
   </si>
   <si>
     <t>SC109390</t>
   </si>
   <si>
-    <t>SC109395</t>
-  </si>
-  <si>
-    <t>SC109405</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>t0712</t>
-  </si>
-  <si>
-    <t>t0712c1</t>
-  </si>
-  <si>
-    <t>SC742313</t>
-  </si>
-  <si>
-    <t>SC742314</t>
-  </si>
-  <si>
-    <t>SC742315</t>
-  </si>
-  <si>
-    <t>t0600</t>
-  </si>
-  <si>
-    <t>t0600c2</t>
-  </si>
-  <si>
-    <t>SC109495</t>
-  </si>
-  <si>
-    <t>SC109514</t>
-  </si>
-  <si>
-    <t>SC109500</t>
-  </si>
-  <si>
-    <t>t0565c1</t>
-  </si>
-  <si>
-    <t>SC109438</t>
-  </si>
-  <si>
-    <t>t0705</t>
-  </si>
-  <si>
-    <t>t0705c1</t>
-  </si>
-  <si>
-    <t>SC742298</t>
-  </si>
-  <si>
-    <t>SC742301</t>
-  </si>
-  <si>
-    <t>SC742299</t>
-  </si>
-  <si>
-    <t>t0750</t>
-  </si>
-  <si>
-    <t>t0750c1</t>
-  </si>
-  <si>
-    <t>SC736755</t>
-  </si>
-  <si>
-    <t>SC736760</t>
-  </si>
-  <si>
-    <t>SC736736</t>
-  </si>
-  <si>
-    <t>t0707</t>
-  </si>
-  <si>
-    <t>t0707c1</t>
-  </si>
-  <si>
-    <t>SC742305</t>
-  </si>
-  <si>
-    <t>SC742306</t>
-  </si>
-  <si>
-    <t>SC742307</t>
-  </si>
-  <si>
-    <t>t0592</t>
-  </si>
-  <si>
-    <t>t0592c1</t>
-  </si>
-  <si>
-    <t>SC109501</t>
-  </si>
-  <si>
-    <t>SC109499</t>
-  </si>
-  <si>
-    <t>SC109498</t>
-  </si>
-  <si>
-    <t>t0679</t>
+    <t>t0749</t>
+  </si>
+  <si>
+    <t>t0749c1</t>
+  </si>
+  <si>
+    <t>SC736820</t>
+  </si>
+  <si>
+    <t>SC736759</t>
+  </si>
+  <si>
+    <t>SC736701</t>
   </si>
   <si>
     <t>t0679c1</t>
@@ -235,346 +556,25 @@
     <t>SC742275</t>
   </si>
   <si>
-    <t>SC742188</t>
-  </si>
-  <si>
-    <t>SC742277</t>
-  </si>
-  <si>
-    <t>t0007</t>
-  </si>
-  <si>
-    <t>t0007c1</t>
-  </si>
-  <si>
-    <t>SC499427</t>
-  </si>
-  <si>
-    <t>SC499423</t>
-  </si>
-  <si>
-    <t>SC499428</t>
-  </si>
-  <si>
-    <t>t0739</t>
-  </si>
-  <si>
-    <t>t0739c1</t>
-  </si>
-  <si>
-    <t>SC736720</t>
-  </si>
-  <si>
-    <t>SC736795</t>
-  </si>
-  <si>
-    <t>SC736726</t>
-  </si>
-  <si>
-    <t>t0575c2</t>
-  </si>
-  <si>
-    <t>SC109406</t>
-  </si>
-  <si>
-    <t>t0243</t>
-  </si>
-  <si>
-    <t>t0243c1</t>
-  </si>
-  <si>
-    <t>SC736787</t>
-  </si>
-  <si>
-    <t>SC736702</t>
-  </si>
-  <si>
-    <t>SC736772</t>
-  </si>
-  <si>
-    <t>t0058</t>
-  </si>
-  <si>
-    <t>t0058c2</t>
-  </si>
-  <si>
-    <t>SC108472</t>
-  </si>
-  <si>
-    <t>SC109353</t>
-  </si>
-  <si>
-    <t>SC109336</t>
-  </si>
-  <si>
-    <t>t0042</t>
-  </si>
-  <si>
-    <t>t0042c1</t>
-  </si>
-  <si>
-    <t>SC253873</t>
-  </si>
-  <si>
-    <t>SC253877</t>
-  </si>
-  <si>
-    <t>SC253872</t>
-  </si>
-  <si>
-    <t>t0766</t>
+    <t>t0483</t>
+  </si>
+  <si>
+    <t>t0483c2</t>
+  </si>
+  <si>
+    <t>SC742320</t>
+  </si>
+  <si>
+    <t>SC742219</t>
+  </si>
+  <si>
+    <t>SC742321</t>
   </si>
   <si>
     <t>t0766c2</t>
   </si>
   <si>
     <t>SC736756</t>
-  </si>
-  <si>
-    <t>SC736703</t>
-  </si>
-  <si>
-    <t>SC730933</t>
-  </si>
-  <si>
-    <t>t0765</t>
-  </si>
-  <si>
-    <t>t0765c1</t>
-  </si>
-  <si>
-    <t>SC736700</t>
-  </si>
-  <si>
-    <t>SC736738</t>
-  </si>
-  <si>
-    <t>SC736739</t>
-  </si>
-  <si>
-    <t>t0766c1</t>
-  </si>
-  <si>
-    <t>SC742179</t>
-  </si>
-  <si>
-    <t>t0315c2</t>
-  </si>
-  <si>
-    <t>SC260715</t>
-  </si>
-  <si>
-    <t>t0483</t>
-  </si>
-  <si>
-    <t>t0483c2</t>
-  </si>
-  <si>
-    <t>SC742320</t>
-  </si>
-  <si>
-    <t>SC742219</t>
-  </si>
-  <si>
-    <t>SC742321</t>
-  </si>
-  <si>
-    <t>t0623</t>
-  </si>
-  <si>
-    <t>t0623c1</t>
-  </si>
-  <si>
-    <t>SC253881</t>
-  </si>
-  <si>
-    <t>SC253893</t>
-  </si>
-  <si>
-    <t>SC253894</t>
-  </si>
-  <si>
-    <t>t0760</t>
-  </si>
-  <si>
-    <t>t0760c1</t>
-  </si>
-  <si>
-    <t>SC736729</t>
-  </si>
-  <si>
-    <t>SC736824</t>
-  </si>
-  <si>
-    <t>SC736803</t>
-  </si>
-  <si>
-    <t>t0703</t>
-  </si>
-  <si>
-    <t>t0703c1</t>
-  </si>
-  <si>
-    <t>SC742295</t>
-  </si>
-  <si>
-    <t>SC742296</t>
-  </si>
-  <si>
-    <t>SC742297</t>
-  </si>
-  <si>
-    <t>t0271</t>
-  </si>
-  <si>
-    <t>t0271c1</t>
-  </si>
-  <si>
-    <t>SC109417</t>
-  </si>
-  <si>
-    <t>SC109426</t>
-  </si>
-  <si>
-    <t>SC109450</t>
-  </si>
-  <si>
-    <t>t0679c2</t>
-  </si>
-  <si>
-    <t>SC742276</t>
-  </si>
-  <si>
-    <t>t0693</t>
-  </si>
-  <si>
-    <t>t0693c2</t>
-  </si>
-  <si>
-    <t>SC742220</t>
-  </si>
-  <si>
-    <t>SC742221</t>
-  </si>
-  <si>
-    <t>SC742222</t>
-  </si>
-  <si>
-    <t>t0599</t>
-  </si>
-  <si>
-    <t>t0599c1</t>
-  </si>
-  <si>
-    <t>SC736788</t>
-  </si>
-  <si>
-    <t>SC736742</t>
-  </si>
-  <si>
-    <t>SC736743</t>
-  </si>
-  <si>
-    <t>t0617</t>
-  </si>
-  <si>
-    <t>t0617c1</t>
-  </si>
-  <si>
-    <t>SC260701</t>
-  </si>
-  <si>
-    <t>SC260705</t>
-  </si>
-  <si>
-    <t>SC260697</t>
-  </si>
-  <si>
-    <t>t0600c1</t>
-  </si>
-  <si>
-    <t>SC109494</t>
-  </si>
-  <si>
-    <t>t0749</t>
-  </si>
-  <si>
-    <t>t0749c1</t>
-  </si>
-  <si>
-    <t>SC736820</t>
-  </si>
-  <si>
-    <t>SC736759</t>
-  </si>
-  <si>
-    <t>SC736701</t>
-  </si>
-  <si>
-    <t>t0022</t>
-  </si>
-  <si>
-    <t>t0022c1</t>
-  </si>
-  <si>
-    <t>SC742290</t>
-  </si>
-  <si>
-    <t>SC742217</t>
-  </si>
-  <si>
-    <t>SC742218</t>
-  </si>
-  <si>
-    <t>t0280</t>
-  </si>
-  <si>
-    <t>t0280c1</t>
-  </si>
-  <si>
-    <t>SC109512</t>
-  </si>
-  <si>
-    <t>SC109516</t>
-  </si>
-  <si>
-    <t>SC109507</t>
-  </si>
-  <si>
-    <t>t0594</t>
-  </si>
-  <si>
-    <t>t0594c1</t>
-  </si>
-  <si>
-    <t>SC736817</t>
-  </si>
-  <si>
-    <t>SC736753</t>
-  </si>
-  <si>
-    <t>SC736754</t>
-  </si>
-  <si>
-    <t>t0058c1</t>
-  </si>
-  <si>
-    <t>SC109341</t>
-  </si>
-  <si>
-    <t>t0209</t>
-  </si>
-  <si>
-    <t>t0209c1</t>
-  </si>
-  <si>
-    <t>SC742216</t>
-  </si>
-  <si>
-    <t>SC742271</t>
-  </si>
-  <si>
-    <t>SC742272</t>
   </si>
 </sst>
 </file>
@@ -977,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1009,10 +1009,10 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="H3">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1038,13 +1038,13 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G4">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="H4">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -1055,28 +1055,28 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
       <c r="G5">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H5">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1087,28 +1087,28 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="H6">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1134,13 +1134,13 @@
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G7">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="H7">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1166,13 +1166,13 @@
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G8">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>16</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -1192,19 +1192,19 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="H9">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
@@ -1215,28 +1215,28 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G10">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="H10">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>16</v>
@@ -1247,28 +1247,28 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G11">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="H11">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>16</v>
@@ -1279,28 +1279,28 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12">
         <v>62</v>
       </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12">
-        <v>61</v>
-      </c>
       <c r="H12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
@@ -1311,28 +1311,28 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
-        <v>69</v>
-      </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G13">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="H13">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
@@ -1343,28 +1343,28 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
         <v>71</v>
       </c>
-      <c r="C14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
-        <v>74</v>
-      </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G14">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>16</v>
@@ -1375,28 +1375,28 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H15">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>16</v>
@@ -1407,28 +1407,28 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
         <v>80</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G16">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H16">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
@@ -1439,28 +1439,28 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>86</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H17">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>16</v>
@@ -1489,10 +1489,10 @@
         <v>15</v>
       </c>
       <c r="G18">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="H18">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>16</v>
@@ -1518,13 +1518,13 @@
         <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G19">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="H19">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>16</v>
@@ -1535,28 +1535,28 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G20">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H20">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>16</v>
@@ -1567,28 +1567,28 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G21">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="H21">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>16</v>
@@ -1599,28 +1599,28 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G22">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="H22">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>16</v>
@@ -1631,28 +1631,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G23">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>16</v>
@@ -1663,28 +1663,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
         <v>114</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>115</v>
       </c>
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G24">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H24">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>16</v>
@@ -1710,13 +1710,13 @@
         <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G25">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="H25">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>16</v>
@@ -1745,10 +1745,10 @@
         <v>15</v>
       </c>
       <c r="G26">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>16</v>
@@ -1777,10 +1777,10 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="H27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>16</v>
@@ -1809,10 +1809,10 @@
         <v>15</v>
       </c>
       <c r="G28">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="H28">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>16</v>
@@ -1838,13 +1838,13 @@
         <v>140</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G29">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="H29">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>16</v>
@@ -1855,28 +1855,28 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
       </c>
       <c r="G30">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="H30">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>16</v>
@@ -1887,28 +1887,28 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
       </c>
       <c r="G31">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H31">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>16</v>
@@ -1919,28 +1919,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G32">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="H32">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>16</v>
@@ -1951,28 +1951,28 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G33">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="H33">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>16</v>
@@ -1983,28 +1983,28 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>164</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G34">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="H34">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>16</v>
@@ -2015,28 +2015,28 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
       </c>
       <c r="G35">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="H35">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>16</v>
@@ -2047,25 +2047,25 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="E36" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G36">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H36">
         <v>12</v>
@@ -2079,28 +2079,28 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E37" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F37" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G37">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>16</v>
@@ -2111,28 +2111,28 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D38" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="F38" t="s">
         <v>15</v>
       </c>
       <c r="G38">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="H38">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>16</v>
@@ -2143,28 +2143,28 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C39" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>183</v>
       </c>
       <c r="E39" t="s">
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G39">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="H39">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>16</v>
@@ -2175,28 +2175,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C40" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D40" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="E40" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="G40">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="H40">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update cgr_summary.xlsx with the latest output under old_output
</commit_message>
<xml_diff>
--- a/cgr_summary.xlsx
+++ b/cgr_summary.xlsx
@@ -46,6 +46,393 @@
     <t>JIGV_Strelka</t>
   </si>
   <si>
+    <t>t0042</t>
+  </si>
+  <si>
+    <t>t0042c1</t>
+  </si>
+  <si>
+    <t>SC253873</t>
+  </si>
+  <si>
+    <t>SC253877</t>
+  </si>
+  <si>
+    <t>SC253872</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>JIGV HTML</t>
+  </si>
+  <si>
+    <t>t0666</t>
+  </si>
+  <si>
+    <t>t0666c1</t>
+  </si>
+  <si>
+    <t>SC502245</t>
+  </si>
+  <si>
+    <t>SC502256</t>
+  </si>
+  <si>
+    <t>SC502234</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>t0705</t>
+  </si>
+  <si>
+    <t>t0705c1</t>
+  </si>
+  <si>
+    <t>SC742298</t>
+  </si>
+  <si>
+    <t>SC742301</t>
+  </si>
+  <si>
+    <t>SC742299</t>
+  </si>
+  <si>
+    <t>t0750</t>
+  </si>
+  <si>
+    <t>t0750c1</t>
+  </si>
+  <si>
+    <t>SC736755</t>
+  </si>
+  <si>
+    <t>SC736760</t>
+  </si>
+  <si>
+    <t>SC736736</t>
+  </si>
+  <si>
+    <t>t0594</t>
+  </si>
+  <si>
+    <t>t0594c1</t>
+  </si>
+  <si>
+    <t>SC736817</t>
+  </si>
+  <si>
+    <t>SC736753</t>
+  </si>
+  <si>
+    <t>SC736754</t>
+  </si>
+  <si>
+    <t>t0592</t>
+  </si>
+  <si>
+    <t>t0592c1</t>
+  </si>
+  <si>
+    <t>SC109501</t>
+  </si>
+  <si>
+    <t>SC109499</t>
+  </si>
+  <si>
+    <t>SC109498</t>
+  </si>
+  <si>
+    <t>t0693</t>
+  </si>
+  <si>
+    <t>t0693c2</t>
+  </si>
+  <si>
+    <t>SC742220</t>
+  </si>
+  <si>
+    <t>SC742221</t>
+  </si>
+  <si>
+    <t>SC742222</t>
+  </si>
+  <si>
+    <t>t0315</t>
+  </si>
+  <si>
+    <t>t0315c2</t>
+  </si>
+  <si>
+    <t>SC260715</t>
+  </si>
+  <si>
+    <t>SC260727</t>
+  </si>
+  <si>
+    <t>SC260729</t>
+  </si>
+  <si>
+    <t>t0575</t>
+  </si>
+  <si>
+    <t>t0575c1</t>
+  </si>
+  <si>
+    <t>SC109390</t>
+  </si>
+  <si>
+    <t>SC109395</t>
+  </si>
+  <si>
+    <t>SC109405</t>
+  </si>
+  <si>
+    <t>t0766</t>
+  </si>
+  <si>
+    <t>t0766c2</t>
+  </si>
+  <si>
+    <t>SC736756</t>
+  </si>
+  <si>
+    <t>SC736703</t>
+  </si>
+  <si>
+    <t>SC730933</t>
+  </si>
+  <si>
+    <t>t0271</t>
+  </si>
+  <si>
+    <t>t0271c1</t>
+  </si>
+  <si>
+    <t>SC109417</t>
+  </si>
+  <si>
+    <t>SC109426</t>
+  </si>
+  <si>
+    <t>SC109450</t>
+  </si>
+  <si>
+    <t>t0600</t>
+  </si>
+  <si>
+    <t>t0600c1</t>
+  </si>
+  <si>
+    <t>SC109494</t>
+  </si>
+  <si>
+    <t>SC109514</t>
+  </si>
+  <si>
+    <t>SC109500</t>
+  </si>
+  <si>
+    <t>t0140</t>
+  </si>
+  <si>
+    <t>t0140c1</t>
+  </si>
+  <si>
+    <t>SC742196</t>
+  </si>
+  <si>
+    <t>SC742286</t>
+  </si>
+  <si>
+    <t>SC742197</t>
+  </si>
+  <si>
+    <t>t0712</t>
+  </si>
+  <si>
+    <t>t0712c1</t>
+  </si>
+  <si>
+    <t>SC742313</t>
+  </si>
+  <si>
+    <t>SC742314</t>
+  </si>
+  <si>
+    <t>SC742315</t>
+  </si>
+  <si>
+    <t>t0565</t>
+  </si>
+  <si>
+    <t>t0565c1</t>
+  </si>
+  <si>
+    <t>SC109438</t>
+  </si>
+  <si>
+    <t>SC109373</t>
+  </si>
+  <si>
+    <t>SC109368</t>
+  </si>
+  <si>
+    <t>t0703</t>
+  </si>
+  <si>
+    <t>t0703c1</t>
+  </si>
+  <si>
+    <t>SC742295</t>
+  </si>
+  <si>
+    <t>SC742296</t>
+  </si>
+  <si>
+    <t>SC742297</t>
+  </si>
+  <si>
+    <t>t0483</t>
+  </si>
+  <si>
+    <t>t0483c2</t>
+  </si>
+  <si>
+    <t>SC742320</t>
+  </si>
+  <si>
+    <t>SC742219</t>
+  </si>
+  <si>
+    <t>SC742321</t>
+  </si>
+  <si>
+    <t>t0022</t>
+  </si>
+  <si>
+    <t>t0022c1</t>
+  </si>
+  <si>
+    <t>SC742290</t>
+  </si>
+  <si>
+    <t>SC742217</t>
+  </si>
+  <si>
+    <t>SC742218</t>
+  </si>
+  <si>
+    <t>t0765</t>
+  </si>
+  <si>
+    <t>t0765c1</t>
+  </si>
+  <si>
+    <t>SC736700</t>
+  </si>
+  <si>
+    <t>SC736738</t>
+  </si>
+  <si>
+    <t>SC736739</t>
+  </si>
+  <si>
+    <t>t0766c1</t>
+  </si>
+  <si>
+    <t>SC742179</t>
+  </si>
+  <si>
+    <t>t0739</t>
+  </si>
+  <si>
+    <t>t0739c1</t>
+  </si>
+  <si>
+    <t>SC736720</t>
+  </si>
+  <si>
+    <t>SC736795</t>
+  </si>
+  <si>
+    <t>SC736726</t>
+  </si>
+  <si>
+    <t>t0575c2</t>
+  </si>
+  <si>
+    <t>SC109406</t>
+  </si>
+  <si>
+    <t>t0679</t>
+  </si>
+  <si>
+    <t>t0679c1</t>
+  </si>
+  <si>
+    <t>SC742275</t>
+  </si>
+  <si>
+    <t>SC742188</t>
+  </si>
+  <si>
+    <t>SC742277</t>
+  </si>
+  <si>
+    <t>t0617</t>
+  </si>
+  <si>
+    <t>t0617c1</t>
+  </si>
+  <si>
+    <t>SC260701</t>
+  </si>
+  <si>
+    <t>SC260705</t>
+  </si>
+  <si>
+    <t>SC260697</t>
+  </si>
+  <si>
+    <t>t0599</t>
+  </si>
+  <si>
+    <t>t0599c1</t>
+  </si>
+  <si>
+    <t>SC736788</t>
+  </si>
+  <si>
+    <t>SC736742</t>
+  </si>
+  <si>
+    <t>SC736743</t>
+  </si>
+  <si>
+    <t>t0679c2</t>
+  </si>
+  <si>
+    <t>SC742276</t>
+  </si>
+  <si>
+    <t>t0058</t>
+  </si>
+  <si>
+    <t>t0058c2</t>
+  </si>
+  <si>
+    <t>SC108472</t>
+  </si>
+  <si>
+    <t>SC109353</t>
+  </si>
+  <si>
+    <t>SC109336</t>
+  </si>
+  <si>
     <t>t0007</t>
   </si>
   <si>
@@ -61,25 +448,73 @@
     <t>SC499428</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>JIGV HTML</t>
-  </si>
-  <si>
-    <t>t0617</t>
-  </si>
-  <si>
-    <t>t0617c1</t>
-  </si>
-  <si>
-    <t>SC260701</t>
-  </si>
-  <si>
-    <t>SC260705</t>
-  </si>
-  <si>
-    <t>SC260697</t>
+    <t>t0058c1</t>
+  </si>
+  <si>
+    <t>SC109341</t>
+  </si>
+  <si>
+    <t>t0565c2</t>
+  </si>
+  <si>
+    <t>SC109437</t>
+  </si>
+  <si>
+    <t>t0749</t>
+  </si>
+  <si>
+    <t>t0749c1</t>
+  </si>
+  <si>
+    <t>SC736820</t>
+  </si>
+  <si>
+    <t>SC736759</t>
+  </si>
+  <si>
+    <t>SC736701</t>
+  </si>
+  <si>
+    <t>t0315c1</t>
+  </si>
+  <si>
+    <t>SC260714</t>
+  </si>
+  <si>
+    <t>t0280</t>
+  </si>
+  <si>
+    <t>t0280c1</t>
+  </si>
+  <si>
+    <t>SC109512</t>
+  </si>
+  <si>
+    <t>SC109516</t>
+  </si>
+  <si>
+    <t>SC109507</t>
+  </si>
+  <si>
+    <t>t0600c2</t>
+  </si>
+  <si>
+    <t>SC109495</t>
+  </si>
+  <si>
+    <t>t0209</t>
+  </si>
+  <si>
+    <t>t0209c1</t>
+  </si>
+  <si>
+    <t>SC742216</t>
+  </si>
+  <si>
+    <t>SC742271</t>
+  </si>
+  <si>
+    <t>SC742272</t>
   </si>
   <si>
     <t>t0243</t>
@@ -97,79 +532,19 @@
     <t>SC736772</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>t0058</t>
-  </si>
-  <si>
-    <t>t0058c1</t>
-  </si>
-  <si>
-    <t>SC109341</t>
-  </si>
-  <si>
-    <t>SC109353</t>
-  </si>
-  <si>
-    <t>SC109336</t>
-  </si>
-  <si>
-    <t>t0712</t>
-  </si>
-  <si>
-    <t>t0712c1</t>
-  </si>
-  <si>
-    <t>SC742313</t>
-  </si>
-  <si>
-    <t>SC742314</t>
-  </si>
-  <si>
-    <t>SC742315</t>
-  </si>
-  <si>
-    <t>t0565</t>
-  </si>
-  <si>
-    <t>t0565c2</t>
-  </si>
-  <si>
-    <t>SC109437</t>
-  </si>
-  <si>
-    <t>SC109373</t>
-  </si>
-  <si>
-    <t>SC109368</t>
-  </si>
-  <si>
-    <t>t0693</t>
-  </si>
-  <si>
-    <t>t0693c2</t>
-  </si>
-  <si>
-    <t>SC742220</t>
-  </si>
-  <si>
-    <t>SC742221</t>
-  </si>
-  <si>
-    <t>SC742222</t>
-  </si>
-  <si>
-    <t>t0058c2</t>
-  </si>
-  <si>
-    <t>SC108472</t>
-  </si>
-  <si>
-    <t>t0565c1</t>
-  </si>
-  <si>
-    <t>SC109438</t>
+    <t>t0707</t>
+  </si>
+  <si>
+    <t>t0707c1</t>
+  </si>
+  <si>
+    <t>SC742305</t>
+  </si>
+  <si>
+    <t>SC742306</t>
+  </si>
+  <si>
+    <t>SC742307</t>
   </si>
   <si>
     <t>t0760</t>
@@ -187,111 +562,6 @@
     <t>SC736803</t>
   </si>
   <si>
-    <t>t0592</t>
-  </si>
-  <si>
-    <t>t0592c1</t>
-  </si>
-  <si>
-    <t>SC109501</t>
-  </si>
-  <si>
-    <t>SC109499</t>
-  </si>
-  <si>
-    <t>SC109498</t>
-  </si>
-  <si>
-    <t>t0750</t>
-  </si>
-  <si>
-    <t>t0750c1</t>
-  </si>
-  <si>
-    <t>SC736755</t>
-  </si>
-  <si>
-    <t>SC736760</t>
-  </si>
-  <si>
-    <t>SC736736</t>
-  </si>
-  <si>
-    <t>t0707</t>
-  </si>
-  <si>
-    <t>t0707c1</t>
-  </si>
-  <si>
-    <t>SC742305</t>
-  </si>
-  <si>
-    <t>SC742306</t>
-  </si>
-  <si>
-    <t>SC742307</t>
-  </si>
-  <si>
-    <t>t0600</t>
-  </si>
-  <si>
-    <t>t0600c1</t>
-  </si>
-  <si>
-    <t>SC109494</t>
-  </si>
-  <si>
-    <t>SC109514</t>
-  </si>
-  <si>
-    <t>SC109500</t>
-  </si>
-  <si>
-    <t>t0140</t>
-  </si>
-  <si>
-    <t>t0140c1</t>
-  </si>
-  <si>
-    <t>SC742196</t>
-  </si>
-  <si>
-    <t>SC742286</t>
-  </si>
-  <si>
-    <t>SC742197</t>
-  </si>
-  <si>
-    <t>t0315</t>
-  </si>
-  <si>
-    <t>t0315c2</t>
-  </si>
-  <si>
-    <t>SC260715</t>
-  </si>
-  <si>
-    <t>SC260727</t>
-  </si>
-  <si>
-    <t>SC260729</t>
-  </si>
-  <si>
-    <t>t0599</t>
-  </si>
-  <si>
-    <t>t0599c1</t>
-  </si>
-  <si>
-    <t>SC736788</t>
-  </si>
-  <si>
-    <t>SC736742</t>
-  </si>
-  <si>
-    <t>SC736743</t>
-  </si>
-  <si>
     <t>t0623</t>
   </si>
   <si>
@@ -305,276 +575,6 @@
   </si>
   <si>
     <t>SC253894</t>
-  </si>
-  <si>
-    <t>t0600c2</t>
-  </si>
-  <si>
-    <t>SC109495</t>
-  </si>
-  <si>
-    <t>t0315c1</t>
-  </si>
-  <si>
-    <t>SC260714</t>
-  </si>
-  <si>
-    <t>t0209</t>
-  </si>
-  <si>
-    <t>t0209c1</t>
-  </si>
-  <si>
-    <t>SC742216</t>
-  </si>
-  <si>
-    <t>SC742271</t>
-  </si>
-  <si>
-    <t>SC742272</t>
-  </si>
-  <si>
-    <t>t0703</t>
-  </si>
-  <si>
-    <t>t0703c1</t>
-  </si>
-  <si>
-    <t>SC742295</t>
-  </si>
-  <si>
-    <t>SC742296</t>
-  </si>
-  <si>
-    <t>SC742297</t>
-  </si>
-  <si>
-    <t>t0666</t>
-  </si>
-  <si>
-    <t>t0666c1</t>
-  </si>
-  <si>
-    <t>SC502245</t>
-  </si>
-  <si>
-    <t>SC502256</t>
-  </si>
-  <si>
-    <t>SC502234</t>
-  </si>
-  <si>
-    <t>t0594</t>
-  </si>
-  <si>
-    <t>t0594c1</t>
-  </si>
-  <si>
-    <t>SC736817</t>
-  </si>
-  <si>
-    <t>SC736753</t>
-  </si>
-  <si>
-    <t>SC736754</t>
-  </si>
-  <si>
-    <t>t0271</t>
-  </si>
-  <si>
-    <t>t0271c1</t>
-  </si>
-  <si>
-    <t>SC109417</t>
-  </si>
-  <si>
-    <t>SC109426</t>
-  </si>
-  <si>
-    <t>SC109450</t>
-  </si>
-  <si>
-    <t>t0022</t>
-  </si>
-  <si>
-    <t>t0022c1</t>
-  </si>
-  <si>
-    <t>SC742290</t>
-  </si>
-  <si>
-    <t>SC742217</t>
-  </si>
-  <si>
-    <t>SC742218</t>
-  </si>
-  <si>
-    <t>t0280</t>
-  </si>
-  <si>
-    <t>t0280c1</t>
-  </si>
-  <si>
-    <t>SC109512</t>
-  </si>
-  <si>
-    <t>SC109516</t>
-  </si>
-  <si>
-    <t>SC109507</t>
-  </si>
-  <si>
-    <t>t0575</t>
-  </si>
-  <si>
-    <t>t0575c2</t>
-  </si>
-  <si>
-    <t>SC109406</t>
-  </si>
-  <si>
-    <t>SC109395</t>
-  </si>
-  <si>
-    <t>SC109405</t>
-  </si>
-  <si>
-    <t>t0766</t>
-  </si>
-  <si>
-    <t>t0766c1</t>
-  </si>
-  <si>
-    <t>SC742179</t>
-  </si>
-  <si>
-    <t>SC736703</t>
-  </si>
-  <si>
-    <t>SC730933</t>
-  </si>
-  <si>
-    <t>t0042</t>
-  </si>
-  <si>
-    <t>t0042c1</t>
-  </si>
-  <si>
-    <t>SC253873</t>
-  </si>
-  <si>
-    <t>SC253877</t>
-  </si>
-  <si>
-    <t>SC253872</t>
-  </si>
-  <si>
-    <t>t0739</t>
-  </si>
-  <si>
-    <t>t0739c1</t>
-  </si>
-  <si>
-    <t>SC736720</t>
-  </si>
-  <si>
-    <t>SC736795</t>
-  </si>
-  <si>
-    <t>SC736726</t>
-  </si>
-  <si>
-    <t>t0679</t>
-  </si>
-  <si>
-    <t>t0679c2</t>
-  </si>
-  <si>
-    <t>SC742276</t>
-  </si>
-  <si>
-    <t>SC742188</t>
-  </si>
-  <si>
-    <t>SC742277</t>
-  </si>
-  <si>
-    <t>t0705</t>
-  </si>
-  <si>
-    <t>t0705c1</t>
-  </si>
-  <si>
-    <t>SC742298</t>
-  </si>
-  <si>
-    <t>SC742301</t>
-  </si>
-  <si>
-    <t>SC742299</t>
-  </si>
-  <si>
-    <t>t0765</t>
-  </si>
-  <si>
-    <t>t0765c1</t>
-  </si>
-  <si>
-    <t>SC736700</t>
-  </si>
-  <si>
-    <t>SC736738</t>
-  </si>
-  <si>
-    <t>SC736739</t>
-  </si>
-  <si>
-    <t>t0575c1</t>
-  </si>
-  <si>
-    <t>SC109390</t>
-  </si>
-  <si>
-    <t>t0749</t>
-  </si>
-  <si>
-    <t>t0749c1</t>
-  </si>
-  <si>
-    <t>SC736820</t>
-  </si>
-  <si>
-    <t>SC736759</t>
-  </si>
-  <si>
-    <t>SC736701</t>
-  </si>
-  <si>
-    <t>t0679c1</t>
-  </si>
-  <si>
-    <t>SC742275</t>
-  </si>
-  <si>
-    <t>t0483</t>
-  </si>
-  <si>
-    <t>t0483c2</t>
-  </si>
-  <si>
-    <t>SC742320</t>
-  </si>
-  <si>
-    <t>SC742219</t>
-  </si>
-  <si>
-    <t>SC742321</t>
-  </si>
-  <si>
-    <t>t0766c2</t>
-  </si>
-  <si>
-    <t>SC736756</t>
   </si>
 </sst>
 </file>
@@ -977,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1006,13 +1006,13 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G3">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="H3">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1023,25 +1023,25 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
       <c r="G4">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -1070,13 +1070,13 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1102,13 +1102,13 @@
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1134,13 +1134,13 @@
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1166,7 +1166,7 @@
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <v>90</v>
@@ -1183,28 +1183,28 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H9">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
@@ -1215,28 +1215,28 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G10">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>16</v>
@@ -1247,28 +1247,28 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>16</v>
@@ -1279,28 +1279,28 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>62</v>
+        <v>144</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
@@ -1311,28 +1311,28 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G13">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="H13">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
@@ -1343,28 +1343,28 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G14">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>16</v>
@@ -1375,28 +1375,28 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G15">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>16</v>
@@ -1407,28 +1407,28 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G16">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H16">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
@@ -1439,28 +1439,28 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G17">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>16</v>
@@ -1471,28 +1471,28 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G18">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="H18">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>16</v>
@@ -1503,28 +1503,28 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>16</v>
@@ -1535,25 +1535,25 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="H20">
         <v>13</v>
@@ -1567,28 +1567,28 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
         <v>82</v>
       </c>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21">
-        <v>74</v>
-      </c>
       <c r="H21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>16</v>
@@ -1599,28 +1599,28 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G22">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>16</v>
@@ -1631,28 +1631,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="H23">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>16</v>
@@ -1663,28 +1663,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G24">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="H24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>16</v>
@@ -1695,28 +1695,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G25">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="H25">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>16</v>
@@ -1727,28 +1727,28 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
       </c>
       <c r="G26">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="H26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>16</v>
@@ -1759,28 +1759,28 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G27">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>16</v>
@@ -1791,28 +1791,28 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H28">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>16</v>
@@ -1823,28 +1823,28 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H29">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>16</v>
@@ -1855,28 +1855,28 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G30">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H30">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>16</v>
@@ -1887,28 +1887,28 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
         <v>146</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>147</v>
       </c>
-      <c r="C31" t="s">
-        <v>148</v>
-      </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G31">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="H31">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>16</v>
@@ -1919,28 +1919,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" t="s">
         <v>151</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>152</v>
       </c>
-      <c r="C32" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" t="s">
-        <v>155</v>
-      </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G32">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="H32">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>16</v>
@@ -1951,28 +1951,28 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G33">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="H33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>16</v>
@@ -1983,28 +1983,28 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E34" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G34">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="H34">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>16</v>
@@ -2015,25 +2015,25 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
       <c r="E35" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G35">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="H35">
         <v>13</v>
@@ -2047,28 +2047,28 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="E36" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G36">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="H36">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>16</v>
@@ -2079,28 +2079,28 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G37">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H37">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>16</v>
@@ -2111,28 +2111,28 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G38">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>16</v>
@@ -2143,28 +2143,28 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" t="s">
         <v>180</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
         <v>181</v>
       </c>
-      <c r="C39" t="s">
-        <v>182</v>
-      </c>
-      <c r="D39" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" t="s">
-        <v>184</v>
-      </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G39">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>16</v>
@@ -2175,28 +2175,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" t="s">
         <v>185</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>186</v>
       </c>
-      <c r="D40" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" t="s">
-        <v>145</v>
-      </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G40">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="H40">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>16</v>

</xml_diff>